<commit_message>
Added processed 2020 DrillingInfo data files
</commit_message>
<xml_diff>
--- a/AnalysisCode_python/Outputs/AF_SAN JOAQUIN.xlsx
+++ b/AnalysisCode_python/Outputs/AF_SAN JOAQUIN.xlsx
@@ -473,25 +473,25 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.08577441745141472</v>
+        <v>0.08577480045838715</v>
       </c>
       <c r="B2" t="n">
-        <v>2.174006110764831e-05</v>
+        <v>2.164722947286865e-05</v>
       </c>
       <c r="C2" t="n">
-        <v>0.000162948933942693</v>
+        <v>0.0001623631487169474</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002442015607692492</v>
+        <v>0.002441401386831815</v>
       </c>
       <c r="F2" t="n">
-        <v>0.002442015607692492</v>
+        <v>0.002441401386831815</v>
       </c>
       <c r="G2" t="n">
-        <v>6.674837417298051e-06</v>
+        <v>6.709801498841058e-06</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -500,36 +500,36 @@
         <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>6.823088297645762e-05</v>
+        <v>6.823181896425233e-05</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4162345301337279</v>
+        <v>0.4162759586104762</v>
       </c>
       <c r="L2" t="n">
-        <v>0.3137411407772357</v>
+        <v>0.3135813319685529</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.0860122695045463</v>
+        <v>0.08601223961811839</v>
       </c>
       <c r="B3" t="n">
-        <v>1.264637177508539e-05</v>
+        <v>1.262576272061368e-05</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0001018191745804025</v>
+        <v>0.0001017868955311419</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00236771658829384</v>
+        <v>0.002367804905851971</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00236771658829384</v>
+        <v>0.002367804905851971</v>
       </c>
       <c r="G3" t="n">
-        <v>7.526483774624894e-06</v>
+        <v>7.559741294690838e-06</v>
       </c>
       <c r="H3" t="n">
         <v>0</v>
@@ -538,36 +538,36 @@
         <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>6.84801249102862e-05</v>
+        <v>6.848015826934183e-05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.3658661601405502</v>
+        <v>0.3660179233335353</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3374102450167918</v>
+        <v>0.3370722261205645</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.08406370400991774</v>
+        <v>0.08405150943884418</v>
       </c>
       <c r="B4" t="n">
-        <v>8.714498979837665e-05</v>
+        <v>8.712342411095218e-05</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0006026151030579259</v>
+        <v>0.0006020147766574068</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0.002976399606072423</v>
+        <v>0.002975551502954534</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002976399606072423</v>
+        <v>0.002975551502954534</v>
       </c>
       <c r="G4" t="n">
-        <v>5.495050869728859e-07</v>
+        <v>5.410902424588396e-07</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -576,13 +576,13 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>6.643824961142456e-05</v>
+        <v>6.642941663624273e-05</v>
       </c>
       <c r="K4" t="n">
-        <v>0.7785011006306489</v>
+        <v>0.781039803591462</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1435048353188785</v>
+        <v>0.1430886172073672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>